<commit_message>
side bar test fixes
</commit_message>
<xml_diff>
--- a/Resources/user_data.xlsx
+++ b/Resources/user_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saurav.tuladhar/Automation/ZconnectWeb/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60815E4F-2FC5-F140-881A-EC21B967B65E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2FE5BF-8EB5-164D-AF0A-9CBDE68F1D7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="139">
   <si>
     <t>Url</t>
   </si>
@@ -414,7 +414,34 @@
     <t>Campaign Messages, Recommendations</t>
   </si>
   <si>
-    <t>Privacy Policy, Terms and Condition</t>
+    <t>Privacy Policy, Terms &amp; Condition</t>
+  </si>
+  <si>
+    <t>Headings</t>
+  </si>
+  <si>
+    <t>/help</t>
+  </si>
+  <si>
+    <t>/videos-screen</t>
+  </si>
+  <si>
+    <t>/services</t>
+  </si>
+  <si>
+    <t>Notifications, Notifications</t>
+  </si>
+  <si>
+    <t>Balance Bills</t>
+  </si>
+  <si>
+    <t>/balanced-bill</t>
+  </si>
+  <si>
+    <t>/notifications, /recommendations</t>
+  </si>
+  <si>
+    <t>chat?question=Hi&amp;user=zConnect%20AI</t>
   </si>
 </sst>
 </file>
@@ -8643,59 +8670,91 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68DDCE12-E4FA-BC4E-A800-7A71F6512E1E}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>123</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C1" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>116</v>
       </c>
       <c r="B2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C2" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C3" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C4" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>118</v>
       </c>
       <c r="B5" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -8703,25 +8762,46 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>122</v>
       </c>
       <c r="B7" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C7" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>121</v>
       </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" location="/share/document/, /services" display="https://zphad.awsapps.com/workdocs/index.html#/share/document/, /services" xr:uid="{52250118-D963-CA47-A3B6-0E0358487517}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>